<commit_message>
Update delivery contents overview to match TeamCity configurations Update release document with description of the delivery contents
</commit_message>
<xml_diff>
--- a/doc/DikesOvertopping - Bestandenoverzicht.xlsx
+++ b/doc/DikesOvertopping - Bestandenoverzicht.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/hans_dewaal_deltares_nl/Documents/0-Werk-D/11-SITO_PS/WVH10_2_F/4 DikesOvertopping/2 DikesOvertopping release/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\DikesOvertopping\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="354" documentId="13_ncr:1_{3DF9BF45-0E9E-4F32-BB0E-AF6107992EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DA2119A-2D0E-442A-A50D-E35D68C0B8F8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D69C033-09B3-4A71-BE8E-E1E0C4397076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FC8A6799-47B4-42FB-98E8-C42260EFA2CB}"/>
+    <workbookView xWindow="28680" yWindow="-330" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FC8A6799-47B4-42FB-98E8-C42260EFA2CB}"/>
   </bookViews>
   <sheets>
     <sheet name="TC_Builds" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="89">
   <si>
     <t>TC build</t>
   </si>
@@ -209,12 +209,6 @@
   </si>
   <si>
     <t>ja</t>
-  </si>
-  <si>
-    <t>nee?</t>
-  </si>
-  <si>
-    <t>Copie uit 'Overtopping_signed'</t>
   </si>
   <si>
     <t>deels</t>
@@ -449,10 +443,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -755,7 +745,7 @@
   <dimension ref="B1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B1" sqref="B1:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +821,7 @@
         <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
         <v>56</v>
@@ -1036,7 +1026,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M32" sqref="M32"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="3" x14ac:dyDescent="0.25"/>
@@ -1068,13 +1058,13 @@
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1100,12 +1090,12 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>2</v>
@@ -1124,7 +1114,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>4</v>
@@ -1138,7 +1128,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>5</v>
@@ -1158,7 +1148,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>7</v>
@@ -1172,7 +1162,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>8</v>
@@ -1186,7 +1176,7 @@
         <v>9</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>9</v>
@@ -1200,7 +1190,7 @@
         <v>10</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>10</v>
@@ -1214,7 +1204,7 @@
         <v>11</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>11</v>
@@ -1228,15 +1218,15 @@
         <v>17</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="5" t="s">
@@ -1245,10 +1235,10 @@
     </row>
     <row r="18" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>13</v>
@@ -1262,7 +1252,7 @@
         <v>14</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>14</v>
@@ -1270,7 +1260,7 @@
     </row>
     <row r="20" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F20" s="4"/>
       <c r="I20" s="6" t="s">
@@ -1285,7 +1275,7 @@
         <v>16</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>16</v>
@@ -1299,7 +1289,7 @@
         <v>17</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>17</v>
@@ -1307,7 +1297,7 @@
     </row>
     <row r="23" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F23" s="4"/>
       <c r="I23" s="6" t="s">
@@ -1316,7 +1306,7 @@
     </row>
     <row r="24" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F24" s="4"/>
       <c r="I24" s="6" t="s">
@@ -1325,7 +1315,7 @@
     </row>
     <row r="25" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F25" s="4"/>
       <c r="I25" s="6" t="s">
@@ -1334,7 +1324,7 @@
     </row>
     <row r="26" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F26" s="4"/>
       <c r="I26" s="6" t="s">
@@ -1343,7 +1333,7 @@
     </row>
     <row r="27" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="5" t="s">
@@ -1352,7 +1342,7 @@
     </row>
     <row r="28" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F28" s="4"/>
       <c r="H28" s="6" t="s">
@@ -1367,7 +1357,7 @@
         <v>14</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>14</v>
@@ -1375,7 +1365,7 @@
     </row>
     <row r="30" spans="1:9" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F30" s="4"/>
       <c r="I30" s="6" t="s">
@@ -1390,7 +1380,7 @@
         <v>16</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>16</v>
@@ -1404,7 +1394,7 @@
         <v>17</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>17</v>
@@ -1412,7 +1402,7 @@
     </row>
     <row r="33" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F33" s="4"/>
       <c r="I33" s="6" t="s">
@@ -1421,7 +1411,7 @@
     </row>
     <row r="34" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F34" s="4"/>
       <c r="I34" s="6" t="s">
@@ -1430,7 +1420,7 @@
     </row>
     <row r="35" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F35" s="4"/>
       <c r="I35" s="6" t="s">
@@ -1439,7 +1429,7 @@
     </row>
     <row r="36" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F36" s="4"/>
       <c r="I36" s="6" t="s">
@@ -1448,12 +1438,12 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C38" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1461,13 +1451,13 @@
         <v>26</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1475,13 +1465,13 @@
         <v>26</v>
       </c>
       <c r="E40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1489,13 +1479,13 @@
         <v>26</v>
       </c>
       <c r="E41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1503,13 +1493,13 @@
         <v>26</v>
       </c>
       <c r="E42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1517,13 +1507,13 @@
         <v>26</v>
       </c>
       <c r="E43" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1531,18 +1521,18 @@
         <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="C45" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F45" s="4"/>
     </row>
@@ -1551,13 +1541,13 @@
         <v>26</v>
       </c>
       <c r="E46" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1565,13 +1555,13 @@
         <v>26</v>
       </c>
       <c r="E47" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1579,13 +1569,13 @@
         <v>26</v>
       </c>
       <c r="E48" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1593,13 +1583,13 @@
         <v>26</v>
       </c>
       <c r="E49" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1607,18 +1597,18 @@
         <v>26</v>
       </c>
       <c r="E50" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1626,15 +1616,15 @@
         <v>26</v>
       </c>
       <c r="E52" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J52" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C53" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>2</v>
@@ -1642,7 +1632,7 @@
     </row>
     <row r="54" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="D54" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1653,7 +1643,7 @@
         <v>32</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>32</v>
@@ -1661,7 +1651,7 @@
     </row>
     <row r="56" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="5" t="s">
@@ -1670,7 +1660,7 @@
     </row>
     <row r="57" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1681,7 +1671,7 @@
         <v>32</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>32</v>
@@ -1689,7 +1679,7 @@
     </row>
     <row r="59" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="D59" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F59" s="4"/>
     </row>
@@ -1701,7 +1691,7 @@
         <v>33</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>33</v>
@@ -1712,13 +1702,13 @@
         <v>26</v>
       </c>
       <c r="E61" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1726,13 +1716,13 @@
         <v>26</v>
       </c>
       <c r="E62" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J62" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:11" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1740,18 +1730,18 @@
         <v>26</v>
       </c>
       <c r="E63" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J63" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C64" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="5" t="s">
@@ -1760,7 +1750,7 @@
     </row>
     <row r="65" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="D65" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="1:10" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1771,7 +1761,7 @@
         <v>32</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H66" s="6" t="s">
         <v>32</v>
@@ -1779,7 +1769,7 @@
     </row>
     <row r="67" spans="1:10" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="D67" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F67" s="4"/>
     </row>
@@ -1791,7 +1781,7 @@
         <v>33</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>33</v>
@@ -1802,13 +1792,13 @@
         <v>26</v>
       </c>
       <c r="E69" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:10" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1816,13 +1806,13 @@
         <v>26</v>
       </c>
       <c r="E70" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J70" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:10" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -1830,13 +1820,13 @@
         <v>26</v>
       </c>
       <c r="E71" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>